<commit_message>
memory allocation check added!
</commit_message>
<xml_diff>
--- a/project/fileXchanger.xlsx
+++ b/project/fileXchanger.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D0B19D-0A57-4E15-9D81-1D8645E6CAB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED9A8AC-C610-499D-96BD-B4AEAE855D26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16470" yWindow="2715" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
   <si>
     <t>file_id[7:0]</t>
   </si>
@@ -93,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,14 +101,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -289,26 +308,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -325,18 +333,40 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -617,14 +647,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
     <col min="5" max="6" width="20.7109375" style="1" customWidth="1"/>
   </cols>
@@ -632,50 +662,50 @@
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3"/>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -697,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BA4884-A89A-4CDA-A0A0-493F10107228}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,73 +744,73 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="17" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="18" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>